<commit_message>
I finished the computation cost analysis, wrote a conclusion for dual quaterions (matrices definitely have the computation edge over dual quaternions simply because dual quaternions have the handicap of needing to be converted to 4x4 matrices before transforming vectors), and converted this latest version to a pdf.
</commit_message>
<xml_diff>
--- a/Quaternion, Dual Numbers, and Dual Quaternions/Computation costs.xlsx
+++ b/Quaternion, Dual Numbers, and Dual Quaternions/Computation costs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Simple_Game_Engine_2\Quaternion, Dual Numbers, and Dual Quaternions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\My_Dual_Quaternion_Paper\Quaternion, Dual Numbers, and Dual Quaternions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20880" windowHeight="8610"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20880" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,16 +1054,75 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>4</v>
+      </c>
       <c r="P29">
         <v>8</v>
       </c>
       <c r="Q29" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f>SUM(G29:G35)</f>
+        <v>26</v>
+      </c>
+      <c r="I36">
+        <f>SUM(I30:I35)</f>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>